<commit_message>
implement logging global level
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aajtechonline-my.sharepoint.com/personal/usman_habeeb_followoz_com/Documents/Documents/UiPath/REFProj/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asif.Islam\Documents\UiPath\GetCustomerData\REFProj\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{96902286-4E3C-425E-A0BF-F83C72A8C5F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E82F198D-7FAD-4A3E-918F-3ADDA29277E0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0865446B-0B4A-4ABC-8D75-37502CA03154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -167,19 +167,67 @@
     <t>OrchestratorQueueName</t>
   </si>
   <si>
-    <t>DB_Connection</t>
-  </si>
-  <si>
-    <t>Data Source=EWORXLAP-128;Initial Catalog=hardrock;Integrated Security=True;</t>
-  </si>
-  <si>
-    <t>SELECT * FROM LogEntries</t>
-  </si>
-  <si>
-    <t>DB_Insert_Table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DB_Query_Table   </t>
+    <t>LogLevel</t>
+  </si>
+  <si>
+    <t>Information</t>
+  </si>
+  <si>
+    <t>LogFilePath</t>
+  </si>
+  <si>
+    <t>Data\Logs\ProcessLog.txt</t>
+  </si>
+  <si>
+    <t>EnableExternalLogging</t>
+  </si>
+  <si>
+    <t>ExternalLogEndpoint</t>
+  </si>
+  <si>
+    <t>https://dc.services.visualstudio.com/v2/track</t>
+  </si>
+  <si>
+    <t>LogTimeFormat</t>
+  </si>
+  <si>
+    <t>yyyy-MM-ddTHH:mm:ss.fffZ</t>
+  </si>
+  <si>
+    <t>CorrelationIdPrefix</t>
+  </si>
+  <si>
+    <t>CORR_</t>
+  </si>
+  <si>
+    <t>ProcessName</t>
+  </si>
+  <si>
+    <t>CustomerProcess</t>
+  </si>
+  <si>
+    <t>RetryCount</t>
+  </si>
+  <si>
+    <t>RetryDelaySeconds</t>
+  </si>
+  <si>
+    <t>ConnectionString</t>
+  </si>
+  <si>
+    <t>Data Source=10.20.30.82;Initial Catalog=CustomerDB;User Id=sql.user;Password=Asif@123;Encrypt=False</t>
+  </si>
+  <si>
+    <t>DBProvider</t>
+  </si>
+  <si>
+    <t>System.Data.SqlClient</t>
+  </si>
+  <si>
+    <t>StatusToProcess</t>
+  </si>
+  <si>
+    <t>New</t>
   </si>
 </sst>
 </file>
@@ -565,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -658,30 +706,119 @@
       <c r="A7" t="s">
         <v>47</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" t="s">
         <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{E50981D8-F1BA-42C4-9899-BC7E66CD19C4}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{B763D9D5-C737-4C67-A0C5-570500B30D07}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add Prefix WRB with custom flows and implement the changes discussed with haider
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asif.Islam\Documents\UiPath\GetCustomerData\REFProj\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asif.Islam\Documents\UiPath\GetCustomerData\ReFrameworkTemplates\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0865446B-0B4A-4ABC-8D75-37502CA03154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12DC563-E174-4935-B33C-5BB6946DA7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -228,6 +228,12 @@
   </si>
   <si>
     <t>New</t>
+  </si>
+  <si>
+    <t>InstrumentationKey</t>
+  </si>
+  <si>
+    <t>c97c1158-d2f5-4e66-9cc1-0961733072c9</t>
   </si>
 </sst>
 </file>
@@ -613,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z20"/>
+  <dimension ref="A1:Z21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -809,6 +815,14 @@
       </c>
       <c r="B20" s="2" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented config base retry and improve globle exception handler and pass data to app insight
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asif.Islam\Documents\UiPath\GetCustomerData\ReFrameworkTemplates\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12DC563-E174-4935-B33C-5BB6946DA7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A326CA-A568-405A-B79B-1D127B6AFC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
@@ -234,6 +234,12 @@
   </si>
   <si>
     <t>c97c1158-d2f5-4e66-9cc1-0961733072c9</t>
+  </si>
+  <si>
+    <t>GlobalExceptionMaxRetryCount</t>
+  </si>
+  <si>
+    <t>GlobalExceptionRetryDelayInSec</t>
   </si>
 </sst>
 </file>
@@ -619,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z21"/>
+  <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -781,48 +787,59 @@
       </c>
     </row>
     <row r="16" spans="1:26">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>62</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>65</v>
+        <v>5</v>
+      </c>
+      <c r="B18" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="2">
-        <v>3</v>
+        <v>66</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>69</v>
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -841,7 +858,7 @@
   <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Changes made in global exception handler and Transaction Status flow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asif.Islam\Documents\UiPath\GetCustomerData\ReFrameworkTemplates\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A326CA-A568-405A-B79B-1D127B6AFC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC80D8C5-5D85-4D06-AF45-3BEEC6A7C5F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>ExScreenshotsFolderPath</t>
   </si>
   <si>
-    <t>Exceptions_Screenshots</t>
-  </si>
-  <si>
     <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
   </si>
   <si>
     <t>GlobalExceptionRetryDelayInSec</t>
+  </si>
+  <si>
+    <t>Data\Screenshots</t>
   </si>
 </sst>
 </file>
@@ -627,7 +627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -675,21 +675,21 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -697,42 +697,42 @@
     </row>
     <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
         <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
         <v>49</v>
-      </c>
-      <c r="B8" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -740,39 +740,39 @@
     </row>
     <row r="10" spans="1:26">
       <c r="A10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
         <v>54</v>
-      </c>
-      <c r="B11" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" t="s">
         <v>56</v>
-      </c>
-      <c r="B12" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
         <v>58</v>
-      </c>
-      <c r="B13" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -780,7 +780,7 @@
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15">
         <v>5</v>
@@ -788,18 +788,18 @@
     </row>
     <row r="16" spans="1:26">
       <c r="A16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -812,23 +812,23 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -836,7 +836,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22">
         <v>5</v>
@@ -857,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -911,18 +911,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -933,109 +933,109 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
         <v>39</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1068,7 +1068,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>